<commit_message>
Updates to figures and tables
Updated formatted excel tables and made minor figure adjustments
</commit_message>
<xml_diff>
--- a/docs/All_ves_by_npz_formatted_table.xlsx
+++ b/docs/All_ves_by_npz_formatted_table.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1800" windowWidth="16224" windowHeight="9108" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2400" windowWidth="16224" windowHeight="9108"/>
   </bookViews>
   <sheets>
     <sheet name="All_ves_by_npz_formatted_table" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="42">
   <si>
     <t>Network</t>
   </si>
@@ -140,16 +140,24 @@
   </si>
   <si>
     <t>X2 southwest</t>
+  </si>
+  <si>
+    <t>N vessels total</t>
+  </si>
+  <si>
+    <t>Deployment start 
+(mm/yyyy)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0%"/>
+    <numFmt numFmtId="165" formatCode="mm/yyyy"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -284,8 +292,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -465,8 +486,14 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="18">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -661,6 +688,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -707,14 +745,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -733,12 +769,44 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="18" fillId="33" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -1061,482 +1129,510 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L14"/>
+  <dimension ref="B2:N15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:K14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="7" max="7" width="15.77734375" customWidth="1"/>
+    <col min="2" max="2" width="14.44140625" style="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" style="19"/>
+    <col min="4" max="4" width="27.33203125" style="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.44140625" style="19" customWidth="1"/>
+    <col min="6" max="6" width="8.6640625" style="19" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.77734375" style="19" customWidth="1"/>
+    <col min="9" max="9" width="12.5546875" customWidth="1"/>
+    <col min="10" max="10" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="2" spans="2:14" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C2" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D2" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="G2" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B3" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="20">
+        <v>43299</v>
+      </c>
+      <c r="E3" s="24">
+        <v>35</v>
+      </c>
+      <c r="F3" s="24">
+        <v>364</v>
+      </c>
+      <c r="G3" s="24">
+        <v>10.4</v>
+      </c>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2">
+        <v>208</v>
+      </c>
+      <c r="J3" s="2">
+        <v>41</v>
+      </c>
+      <c r="K3" s="2">
+        <v>14</v>
+      </c>
+      <c r="L3" s="3">
+        <v>0.197115384615384</v>
+      </c>
+      <c r="M3" s="4">
+        <v>0.36585365853658502</v>
+      </c>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B4" s="22"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="20">
+        <v>43435</v>
+      </c>
+      <c r="E4" s="24">
+        <v>71</v>
+      </c>
+      <c r="F4" s="24">
+        <v>395</v>
+      </c>
+      <c r="G4" s="24">
+        <v>5.56</v>
+      </c>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5">
+        <v>216</v>
+      </c>
+      <c r="J4" s="5">
+        <v>33</v>
+      </c>
+      <c r="K4" s="5">
+        <v>0</v>
+      </c>
+      <c r="L4" s="6">
+        <v>0.15277777777777701</v>
+      </c>
+      <c r="M4" s="16">
+        <v>0.66666666666666596</v>
+      </c>
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B5" s="22"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="20">
+        <v>43556</v>
+      </c>
+      <c r="E5" s="24">
+        <v>75</v>
+      </c>
+      <c r="F5" s="24">
+        <v>473</v>
+      </c>
+      <c r="G5" s="24">
+        <v>6.31</v>
+      </c>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5">
+        <v>326</v>
+      </c>
+      <c r="J5" s="5">
+        <v>57</v>
+      </c>
+      <c r="K5" s="5">
+        <v>31</v>
+      </c>
+      <c r="L5" s="6">
+        <v>0.17484662576687099</v>
+      </c>
+      <c r="M5" s="7">
+        <v>0.57894736842105199</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B6" s="22"/>
+      <c r="C6" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="20">
+        <v>43313</v>
+      </c>
+      <c r="E6" s="24">
+        <v>67</v>
+      </c>
+      <c r="F6" s="24">
+        <v>523</v>
+      </c>
+      <c r="G6" s="24">
+        <v>7.81</v>
+      </c>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5">
+        <v>112</v>
+      </c>
+      <c r="J6" s="5">
+        <v>41</v>
+      </c>
+      <c r="K6" s="5">
+        <v>8</v>
+      </c>
+      <c r="L6" s="6">
+        <v>0.36607142857142799</v>
+      </c>
+      <c r="M6" s="7">
+        <v>0.292682926829268</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B7" s="22"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="20">
+        <v>43435</v>
+      </c>
+      <c r="E7" s="24">
+        <v>70</v>
+      </c>
+      <c r="F7" s="24">
+        <v>443</v>
+      </c>
+      <c r="G7" s="24">
+        <v>6.33</v>
+      </c>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5">
+        <v>265</v>
+      </c>
+      <c r="J7" s="5">
+        <v>42</v>
+      </c>
+      <c r="K7" s="5">
+        <v>29</v>
+      </c>
+      <c r="L7" s="6">
+        <v>0.15849056603773501</v>
+      </c>
+      <c r="M7" s="7">
+        <v>0.71428571428571397</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B8" s="25"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="20">
+        <v>43617</v>
+      </c>
+      <c r="E8" s="24">
+        <v>81</v>
+      </c>
+      <c r="F8" s="24">
+        <v>343</v>
+      </c>
+      <c r="G8" s="24">
+        <v>4.2300000000000004</v>
+      </c>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13">
+        <v>241</v>
+      </c>
+      <c r="J8" s="13">
+        <v>75</v>
+      </c>
+      <c r="K8" s="13">
+        <v>65</v>
+      </c>
+      <c r="L8" s="14">
+        <v>0.31120331950207403</v>
+      </c>
+      <c r="M8" s="15">
+        <v>0.90666666666666595</v>
+      </c>
+      <c r="N8" s="1"/>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B9" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="20">
+        <v>44075</v>
+      </c>
+      <c r="E9" s="24">
+        <v>116</v>
+      </c>
+      <c r="F9" s="24">
+        <v>376</v>
+      </c>
+      <c r="G9" s="24">
+        <v>3.24</v>
+      </c>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2">
+        <v>125</v>
+      </c>
+      <c r="J9" s="2">
+        <v>7</v>
+      </c>
+      <c r="K9" s="2">
+        <v>3</v>
+      </c>
+      <c r="L9" s="3">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="M9" s="4">
+        <v>0.42859999999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B10" s="25"/>
+      <c r="C10" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="20">
+        <v>43709</v>
+      </c>
+      <c r="E10" s="24">
+        <v>111</v>
+      </c>
+      <c r="F10" s="24">
+        <v>126</v>
+      </c>
+      <c r="G10" s="24">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13">
+        <v>109</v>
+      </c>
+      <c r="J10" s="13">
+        <v>4</v>
+      </c>
+      <c r="K10" s="13">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="L10" s="14">
+        <v>3.6700000000000003E-2</v>
+      </c>
+      <c r="M10" s="15">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B11" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="20">
+        <v>44562</v>
+      </c>
+      <c r="E11" s="24">
+        <v>91</v>
+      </c>
+      <c r="F11" s="24">
+        <v>575</v>
+      </c>
+      <c r="G11" s="24">
+        <v>6.32</v>
+      </c>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2">
+        <v>390</v>
+      </c>
+      <c r="J11" s="2">
+        <v>1</v>
+      </c>
+      <c r="K11" s="2">
+        <v>0</v>
+      </c>
+      <c r="L11" s="3">
+        <v>2.5999999999999999E-3</v>
+      </c>
+      <c r="M11" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B12" s="22"/>
+      <c r="C12" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="20">
+        <v>44562</v>
+      </c>
+      <c r="E12" s="24">
+        <v>106</v>
+      </c>
+      <c r="F12" s="24">
+        <v>425</v>
+      </c>
+      <c r="G12" s="24">
+        <v>4.01</v>
+      </c>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5">
+        <v>345</v>
+      </c>
+      <c r="J12" s="5">
+        <v>21</v>
+      </c>
+      <c r="K12" s="5">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="L12" s="6">
+        <v>6.0900000000000003E-2</v>
+      </c>
+      <c r="M12" s="7">
+        <v>0.1429</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B13" s="22"/>
+      <c r="C13" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="20">
+        <v>43862</v>
+      </c>
+      <c r="E13" s="24">
+        <v>164</v>
+      </c>
+      <c r="F13" s="24">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="3">
-        <v>201807</v>
-      </c>
-      <c r="D2" s="3">
-        <v>35</v>
-      </c>
-      <c r="E2" s="3">
-        <v>364</v>
-      </c>
-      <c r="F2" s="3">
-        <v>10.4</v>
-      </c>
-      <c r="G2" s="3">
-        <v>208</v>
-      </c>
-      <c r="H2" s="3">
-        <v>39</v>
-      </c>
-      <c r="I2" s="3">
-        <v>14</v>
-      </c>
-      <c r="J2" s="4">
-        <v>0.1875</v>
-      </c>
-      <c r="K2" s="5">
-        <v>0.35899999999999999</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" s="6"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7">
-        <v>201812</v>
-      </c>
-      <c r="D3" s="7">
-        <v>71</v>
-      </c>
-      <c r="E3" s="7">
-        <v>395</v>
-      </c>
-      <c r="F3" s="7">
-        <v>5.56</v>
-      </c>
-      <c r="G3" s="7">
-        <v>95</v>
-      </c>
-      <c r="H3" s="7">
-        <v>1</v>
-      </c>
-      <c r="I3" s="7">
-        <v>0</v>
-      </c>
-      <c r="J3" s="8">
-        <v>1.0500000000000001E-2</v>
-      </c>
-      <c r="K3" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="6"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7">
-        <v>201904</v>
-      </c>
-      <c r="D4" s="7">
-        <v>75</v>
-      </c>
-      <c r="E4" s="7">
-        <v>473</v>
-      </c>
-      <c r="F4" s="7">
-        <v>6.31</v>
-      </c>
-      <c r="G4" s="7">
-        <v>327</v>
-      </c>
-      <c r="H4" s="7">
+      <c r="G13" s="24">
+        <v>0.02</v>
+      </c>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5">
+        <v>2</v>
+      </c>
+      <c r="J13" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="K13" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="L13" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="M13" s="10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B14" s="22"/>
+      <c r="C14" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="20">
+        <v>44571</v>
+      </c>
+      <c r="E14" s="24">
+        <v>85</v>
+      </c>
+      <c r="F14" s="24">
+        <v>343</v>
+      </c>
+      <c r="G14" s="24">
+        <v>4.04</v>
+      </c>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5">
+        <v>264</v>
+      </c>
+      <c r="J14" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="K14" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="L14" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="M14" s="12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B15" s="25"/>
+      <c r="C15" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" s="20">
+        <v>44326</v>
+      </c>
+      <c r="E15" s="24">
+        <v>164</v>
+      </c>
+      <c r="F15" s="24">
+        <v>1109</v>
+      </c>
+      <c r="G15" s="24">
+        <v>6.76</v>
+      </c>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13">
+        <v>831</v>
+      </c>
+      <c r="J15" s="13">
+        <v>61</v>
+      </c>
+      <c r="K15" s="13">
         <v>52</v>
       </c>
-      <c r="I4" s="7">
-        <v>31</v>
-      </c>
-      <c r="J4" s="8">
-        <v>0.159</v>
-      </c>
-      <c r="K4" s="9">
-        <v>0.59619999999999995</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="6"/>
-      <c r="B5" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="7">
-        <v>201808</v>
-      </c>
-      <c r="D5" s="7">
-        <v>67</v>
-      </c>
-      <c r="E5" s="7">
-        <v>523</v>
-      </c>
-      <c r="F5" s="7">
-        <v>7.81</v>
-      </c>
-      <c r="G5" s="7">
-        <v>265</v>
-      </c>
-      <c r="H5" s="7">
-        <v>37</v>
-      </c>
-      <c r="I5" s="7">
-        <v>8</v>
-      </c>
-      <c r="J5" s="8">
-        <v>0.1396</v>
-      </c>
-      <c r="K5" s="9">
-        <v>0.2162</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="6"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7">
-        <v>201812</v>
-      </c>
-      <c r="D6" s="7">
-        <v>70</v>
-      </c>
-      <c r="E6" s="7">
-        <v>443</v>
-      </c>
-      <c r="F6" s="7">
-        <v>6.33</v>
-      </c>
-      <c r="G6" s="7">
-        <v>265</v>
-      </c>
-      <c r="H6" s="7">
-        <v>40</v>
-      </c>
-      <c r="I6" s="7">
-        <v>29</v>
-      </c>
-      <c r="J6" s="8">
-        <v>0.15090000000000001</v>
-      </c>
-      <c r="K6" s="9">
-        <v>0.72499999999999998</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" s="15"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="16">
-        <v>201906</v>
-      </c>
-      <c r="D7" s="16">
-        <v>81</v>
-      </c>
-      <c r="E7" s="16">
-        <v>343</v>
-      </c>
-      <c r="F7" s="16">
-        <v>4.2300000000000004</v>
-      </c>
-      <c r="G7" s="16">
-        <v>241</v>
-      </c>
-      <c r="H7" s="16">
-        <v>72</v>
-      </c>
-      <c r="I7" s="16">
-        <v>65</v>
-      </c>
-      <c r="J7" s="17">
-        <v>0.29880000000000001</v>
-      </c>
-      <c r="K7" s="18">
-        <v>0.90280000000000005</v>
-      </c>
-      <c r="L7" s="1"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="3">
-        <v>202009</v>
-      </c>
-      <c r="D8" s="3">
-        <v>116</v>
-      </c>
-      <c r="E8" s="3">
-        <v>376</v>
-      </c>
-      <c r="F8" s="3">
-        <v>3.24</v>
-      </c>
-      <c r="G8" s="3">
-        <v>125</v>
-      </c>
-      <c r="H8" s="3">
-        <v>7</v>
-      </c>
-      <c r="I8" s="3">
-        <v>3</v>
-      </c>
-      <c r="J8" s="4">
-        <v>5.6000000000000001E-2</v>
-      </c>
-      <c r="K8" s="5">
-        <v>0.42859999999999998</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9" s="15"/>
-      <c r="B9" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="16">
-        <v>201909</v>
-      </c>
-      <c r="D9" s="16">
-        <v>111</v>
-      </c>
-      <c r="E9" s="16">
-        <v>126</v>
-      </c>
-      <c r="F9" s="16">
-        <v>1.1399999999999999</v>
-      </c>
-      <c r="G9" s="16">
-        <v>109</v>
-      </c>
-      <c r="H9" s="16">
-        <v>4</v>
-      </c>
-      <c r="I9" s="16">
-        <v>2</v>
-      </c>
-      <c r="J9" s="17">
-        <v>3.6700000000000003E-2</v>
-      </c>
-      <c r="K9" s="18">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="3">
-        <v>202201</v>
-      </c>
-      <c r="D10" s="3">
-        <v>91</v>
-      </c>
-      <c r="E10" s="3">
-        <v>575</v>
-      </c>
-      <c r="F10" s="3">
-        <v>6.32</v>
-      </c>
-      <c r="G10" s="3">
-        <v>390</v>
-      </c>
-      <c r="H10" s="3">
-        <v>1</v>
-      </c>
-      <c r="I10" s="3">
-        <v>0</v>
-      </c>
-      <c r="J10" s="4">
-        <v>2.5999999999999999E-3</v>
-      </c>
-      <c r="K10" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A11" s="6"/>
-      <c r="B11" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="7">
-        <v>202201</v>
-      </c>
-      <c r="D11" s="7">
-        <v>106</v>
-      </c>
-      <c r="E11" s="7">
-        <v>425</v>
-      </c>
-      <c r="F11" s="7">
-        <v>4.01</v>
-      </c>
-      <c r="G11" s="7">
-        <v>345</v>
-      </c>
-      <c r="H11" s="7">
-        <v>21</v>
-      </c>
-      <c r="I11" s="7">
-        <v>3</v>
-      </c>
-      <c r="J11" s="8">
-        <v>6.0900000000000003E-2</v>
-      </c>
-      <c r="K11" s="9">
-        <v>0.1429</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A12" s="6"/>
-      <c r="B12" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="7">
-        <v>202002</v>
-      </c>
-      <c r="D12" s="7">
-        <v>164</v>
-      </c>
-      <c r="E12" s="7">
-        <v>4</v>
-      </c>
-      <c r="F12" s="7">
-        <v>0.02</v>
-      </c>
-      <c r="G12" s="7">
-        <v>2</v>
-      </c>
-      <c r="H12" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="I12" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="J12" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="K12" s="12" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A13" s="6"/>
-      <c r="B13" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" s="7">
-        <v>202201</v>
-      </c>
-      <c r="D13" s="7">
-        <v>85</v>
-      </c>
-      <c r="E13" s="7">
-        <v>343</v>
-      </c>
-      <c r="F13" s="7">
-        <v>4.04</v>
-      </c>
-      <c r="G13" s="7">
-        <v>264</v>
-      </c>
-      <c r="H13" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="I13" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="J13" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="K13" s="14" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A14" s="15"/>
-      <c r="B14" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" s="16">
-        <v>202105</v>
-      </c>
-      <c r="D14" s="16">
-        <v>164</v>
-      </c>
-      <c r="E14" s="16">
-        <v>1109</v>
-      </c>
-      <c r="F14" s="16">
-        <v>6.76</v>
-      </c>
-      <c r="G14" s="16">
-        <v>831</v>
-      </c>
-      <c r="H14" s="16">
-        <v>61</v>
-      </c>
-      <c r="I14" s="16">
-        <v>52</v>
-      </c>
-      <c r="J14" s="17">
+      <c r="L15" s="14">
         <v>7.3400000000000007E-2</v>
       </c>
-      <c r="K14" s="18">
+      <c r="M15" s="15">
         <v>0.85250000000000004</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="J2:J14">
+  <mergeCells count="5">
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="C6:C8"/>
+    <mergeCell ref="B3:B8"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B11:B15"/>
+  </mergeCells>
+  <conditionalFormatting sqref="L3:L15">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -1548,7 +1644,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K11 K13:K14">
+  <conditionalFormatting sqref="M3:M12 M14:M15">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -1568,8 +1664,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="S10" sqref="S10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1647,42 +1743,42 @@
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="2">
         <v>201807</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2">
         <v>35</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="2">
         <v>364</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="2">
         <v>10.4</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3">
         <v>208</v>
       </c>
-      <c r="G3" s="3">
-        <v>39</v>
-      </c>
-      <c r="H3" s="3">
+      <c r="G3">
+        <v>41</v>
+      </c>
+      <c r="H3" s="2">
         <v>14</v>
       </c>
-      <c r="I3" s="4">
-        <v>0.1875</v>
-      </c>
-      <c r="J3" s="5">
-        <v>0.35899999999999999</v>
+      <c r="I3" s="18">
+        <v>0.197115384615384</v>
+      </c>
+      <c r="J3" s="4">
+        <v>0.36585365853658502</v>
       </c>
       <c r="N3" t="s">
         <v>12</v>
       </c>
       <c r="O3">
         <f>SUM(G3:G5)-SUM(H3:H5)</f>
-        <v>47</v>
+        <v>86</v>
       </c>
       <c r="P3">
         <f>SUM(H3:H5)</f>
@@ -1690,59 +1786,59 @@
       </c>
       <c r="Q3">
         <f>SUM(O3:P3)</f>
-        <v>92</v>
+        <v>131</v>
       </c>
       <c r="S3" t="s">
         <v>12</v>
       </c>
       <c r="T3">
         <f>$Q3/$Q$10*O$10</f>
-        <v>35.15223880597015</v>
+        <v>60.198433420365532</v>
       </c>
       <c r="U3">
         <f>$Q3/$Q$10*P$10</f>
-        <v>56.84776119402985</v>
+        <v>70.801566579634468</v>
       </c>
       <c r="V3">
         <f>SUM(T3:U3)</f>
-        <v>92</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A4" s="7"/>
-      <c r="B4" s="7">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5">
         <v>201812</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="5">
         <v>71</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="5">
         <v>395</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="5">
         <v>5.56</v>
       </c>
-      <c r="F4" s="7">
-        <v>95</v>
-      </c>
-      <c r="G4" s="7">
-        <v>1</v>
-      </c>
-      <c r="H4" s="7">
+      <c r="F4">
+        <v>216</v>
+      </c>
+      <c r="G4">
+        <v>33</v>
+      </c>
+      <c r="H4" s="5">
         <v>0</v>
       </c>
-      <c r="I4" s="8">
-        <v>1.0500000000000001E-2</v>
-      </c>
-      <c r="J4" s="19">
-        <v>0</v>
+      <c r="I4" s="18">
+        <v>0.15277777777777701</v>
+      </c>
+      <c r="J4" s="16">
+        <v>0.66666666666666596</v>
       </c>
       <c r="N4" t="s">
         <v>14</v>
       </c>
       <c r="O4">
         <f>SUM(G6:G8)-SUM(H6:H8)</f>
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="P4">
         <f>SUM(H6:H8)</f>
@@ -1750,52 +1846,52 @@
       </c>
       <c r="Q4">
         <f t="shared" ref="Q4:Q9" si="0">SUM(O4:P4)</f>
-        <v>149</v>
+        <v>158</v>
       </c>
       <c r="S4" t="s">
         <v>14</v>
       </c>
       <c r="T4">
         <f t="shared" ref="T4:U9" si="1">$Q4/$Q$10*O$10</f>
-        <v>56.931343283582088</v>
+        <v>72.605744125326368</v>
       </c>
       <c r="U4">
         <f t="shared" si="1"/>
-        <v>92.068656716417905</v>
+        <v>85.394255874673632</v>
       </c>
       <c r="V4">
         <f t="shared" ref="V4:V9" si="2">SUM(T4:U4)</f>
-        <v>149</v>
+        <v>158</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5">
         <v>201904</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="5">
         <v>75</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="5">
         <v>473</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5" s="5">
         <v>6.31</v>
       </c>
-      <c r="F5" s="7">
-        <v>327</v>
-      </c>
-      <c r="G5" s="7">
-        <v>52</v>
-      </c>
-      <c r="H5" s="7">
+      <c r="F5">
+        <v>326</v>
+      </c>
+      <c r="G5">
+        <v>57</v>
+      </c>
+      <c r="H5" s="5">
         <v>31</v>
       </c>
-      <c r="I5" s="8">
-        <v>0.159</v>
-      </c>
-      <c r="J5" s="9">
-        <v>0.59619999999999995</v>
+      <c r="I5" s="18">
+        <v>0.17484662576687099</v>
+      </c>
+      <c r="J5" s="7">
+        <v>0.57894736842105199</v>
       </c>
       <c r="N5" t="s">
         <v>16</v>
@@ -1815,11 +1911,11 @@
       </c>
       <c r="T5">
         <f t="shared" si="1"/>
-        <v>2.6746268656716419</v>
+        <v>3.2167101827676241</v>
       </c>
       <c r="U5">
         <f t="shared" si="1"/>
-        <v>4.3253731343283581</v>
+        <v>3.7832898172323763</v>
       </c>
       <c r="V5">
         <f t="shared" si="2"/>
@@ -1827,35 +1923,35 @@
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B6" s="5">
         <v>201808</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="5">
         <v>67</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="5">
         <v>523</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="5">
         <v>7.81</v>
       </c>
-      <c r="F6" s="7">
-        <v>265</v>
-      </c>
-      <c r="G6" s="7">
-        <v>37</v>
-      </c>
-      <c r="H6" s="7">
+      <c r="F6">
+        <v>112</v>
+      </c>
+      <c r="G6">
+        <v>41</v>
+      </c>
+      <c r="H6" s="5">
         <v>8</v>
       </c>
-      <c r="I6" s="8">
-        <v>0.1396</v>
-      </c>
-      <c r="J6" s="9">
-        <v>0.2162</v>
+      <c r="I6" s="18">
+        <v>0.36607142857142799</v>
+      </c>
+      <c r="J6" s="7">
+        <v>0.292682926829268</v>
       </c>
       <c r="N6" t="s">
         <v>17</v>
@@ -1875,11 +1971,11 @@
       </c>
       <c r="T6">
         <f t="shared" si="1"/>
-        <v>1.5283582089552239</v>
+        <v>1.8381201044386424</v>
       </c>
       <c r="U6">
         <f t="shared" si="1"/>
-        <v>2.4716417910447763</v>
+        <v>2.1618798955613578</v>
       </c>
       <c r="V6">
         <f t="shared" si="2"/>
@@ -1887,33 +1983,33 @@
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5">
         <v>201812</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="5">
         <v>70</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="5">
         <v>443</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="5">
         <v>6.33</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7">
         <v>265</v>
       </c>
-      <c r="G7" s="7">
-        <v>40</v>
-      </c>
-      <c r="H7" s="7">
+      <c r="G7">
+        <v>42</v>
+      </c>
+      <c r="H7" s="5">
         <v>29</v>
       </c>
-      <c r="I7" s="8">
-        <v>0.15090000000000001</v>
-      </c>
-      <c r="J7" s="9">
-        <v>0.72499999999999998</v>
+      <c r="I7" s="18">
+        <v>0.15849056603773501</v>
+      </c>
+      <c r="J7" s="7">
+        <v>0.71428571428571397</v>
       </c>
       <c r="N7" t="s">
         <v>19</v>
@@ -1933,11 +2029,11 @@
       </c>
       <c r="T7">
         <f t="shared" si="1"/>
-        <v>0.38208955223880597</v>
+        <v>0.45953002610966059</v>
       </c>
       <c r="U7">
         <f t="shared" si="1"/>
-        <v>0.61791044776119408</v>
+        <v>0.54046997389033946</v>
       </c>
       <c r="V7">
         <f t="shared" si="2"/>
@@ -1945,33 +2041,33 @@
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A8" s="16"/>
-      <c r="B8" s="16">
+      <c r="A8" s="13"/>
+      <c r="B8" s="13">
         <v>201906</v>
       </c>
-      <c r="C8" s="16">
+      <c r="C8" s="13">
         <v>81</v>
       </c>
-      <c r="D8" s="16">
+      <c r="D8" s="13">
         <v>343</v>
       </c>
-      <c r="E8" s="16">
+      <c r="E8" s="13">
         <v>4.2300000000000004</v>
       </c>
-      <c r="F8" s="16">
+      <c r="F8">
         <v>241</v>
       </c>
-      <c r="G8" s="16">
-        <v>72</v>
-      </c>
-      <c r="H8" s="16">
+      <c r="G8">
+        <v>75</v>
+      </c>
+      <c r="H8" s="13">
         <v>65</v>
       </c>
-      <c r="I8" s="17">
-        <v>0.29880000000000001</v>
-      </c>
-      <c r="J8" s="18">
-        <v>0.90280000000000005</v>
+      <c r="I8" s="18">
+        <v>0.31120331950207403</v>
+      </c>
+      <c r="J8" s="15">
+        <v>0.90666666666666595</v>
       </c>
       <c r="N8" t="s">
         <v>20</v>
@@ -1991,11 +2087,11 @@
       </c>
       <c r="T8">
         <f t="shared" si="1"/>
-        <v>8.0238805970149247</v>
+        <v>9.6501305483028723</v>
       </c>
       <c r="U8">
         <f t="shared" si="1"/>
-        <v>12.976119402985073</v>
+        <v>11.349869451697129</v>
       </c>
       <c r="V8">
         <f t="shared" si="2"/>
@@ -2003,34 +2099,34 @@
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="2">
         <v>202009</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="2">
         <v>116</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="2">
         <v>376</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="2">
         <v>3.24</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="2">
         <v>125</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G9" s="2">
         <v>7</v>
       </c>
-      <c r="H9" s="3">
+      <c r="H9" s="2">
         <v>3</v>
       </c>
-      <c r="I9" s="4">
+      <c r="I9" s="3">
         <v>5.6000000000000001E-2</v>
       </c>
-      <c r="J9" s="5">
+      <c r="J9" s="4">
         <v>0.42859999999999998</v>
       </c>
       <c r="N9" t="s">
@@ -2051,11 +2147,11 @@
       </c>
       <c r="T9">
         <f t="shared" si="1"/>
-        <v>23.307462686567163</v>
+        <v>28.031331592689295</v>
       </c>
       <c r="U9">
         <f t="shared" si="1"/>
-        <v>37.692537313432837</v>
+        <v>32.968668407310702</v>
       </c>
       <c r="V9">
         <f t="shared" si="2"/>
@@ -2063,39 +2159,39 @@
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="16">
+      <c r="B10" s="13">
         <v>201909</v>
       </c>
-      <c r="C10" s="16">
+      <c r="C10" s="13">
         <v>111</v>
       </c>
-      <c r="D10" s="16">
+      <c r="D10" s="13">
         <v>126</v>
       </c>
-      <c r="E10" s="16">
+      <c r="E10" s="13">
         <v>1.1399999999999999</v>
       </c>
-      <c r="F10" s="16">
+      <c r="F10" s="13">
         <v>109</v>
       </c>
-      <c r="G10" s="16">
+      <c r="G10" s="13">
         <v>4</v>
       </c>
-      <c r="H10" s="16">
+      <c r="H10" s="13">
         <v>2</v>
       </c>
-      <c r="I10" s="17">
+      <c r="I10" s="14">
         <v>3.6700000000000003E-2</v>
       </c>
-      <c r="J10" s="18">
+      <c r="J10" s="15">
         <v>0.5</v>
       </c>
       <c r="O10">
         <f>SUM(O3:O9)</f>
-        <v>128</v>
+        <v>176</v>
       </c>
       <c r="P10">
         <f t="shared" ref="P10:Q10" si="3">SUM(P3:P9)</f>
@@ -2103,189 +2199,189 @@
       </c>
       <c r="Q10">
         <f t="shared" si="3"/>
-        <v>335</v>
+        <v>383</v>
       </c>
       <c r="T10">
         <f>SUM(T3:T9)</f>
-        <v>128</v>
+        <v>176.00000000000003</v>
       </c>
       <c r="U10">
         <f t="shared" ref="U10:V10" si="4">SUM(U3:U9)</f>
-        <v>207</v>
+        <v>206.99999999999997</v>
       </c>
       <c r="V10">
         <f t="shared" si="4"/>
-        <v>335</v>
+        <v>383</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="2">
         <v>202201</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="2">
         <v>91</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="2">
         <v>575</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="2">
         <v>6.32</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F11" s="2">
         <v>390</v>
       </c>
-      <c r="G11" s="3">
+      <c r="G11" s="2">
         <v>1</v>
       </c>
-      <c r="H11" s="3">
+      <c r="H11" s="2">
         <v>0</v>
       </c>
-      <c r="I11" s="4">
+      <c r="I11" s="3">
         <v>2.5999999999999999E-3</v>
       </c>
-      <c r="J11" s="5">
+      <c r="J11" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="7">
+      <c r="B12" s="5">
         <v>202201</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C12" s="5">
         <v>106</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D12" s="5">
         <v>425</v>
       </c>
-      <c r="E12" s="7">
+      <c r="E12" s="5">
         <v>4.01</v>
       </c>
-      <c r="F12" s="7">
+      <c r="F12" s="5">
         <v>345</v>
       </c>
-      <c r="G12" s="7">
+      <c r="G12" s="5">
         <v>21</v>
       </c>
-      <c r="H12" s="7">
+      <c r="H12" s="5">
         <v>3</v>
       </c>
-      <c r="I12" s="8">
+      <c r="I12" s="6">
         <v>6.0900000000000003E-2</v>
       </c>
-      <c r="J12" s="9">
+      <c r="J12" s="7">
         <v>0.1429</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="7">
+      <c r="B13" s="5">
         <v>202002</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C13" s="5">
         <v>164</v>
       </c>
-      <c r="D13" s="7">
+      <c r="D13" s="5">
         <v>4</v>
       </c>
-      <c r="E13" s="7">
+      <c r="E13" s="5">
         <v>0.02</v>
       </c>
-      <c r="F13" s="7">
+      <c r="F13" s="5">
         <v>2</v>
       </c>
-      <c r="G13" s="10" t="s">
+      <c r="G13" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="H13" s="10" t="s">
+      <c r="H13" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="I13" s="11" t="s">
+      <c r="I13" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="J13" s="12" t="s">
+      <c r="J13" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="R13" s="20" t="s">
+      <c r="R13" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="S13" s="20">
+      <c r="S13" s="17">
         <f>_xlfn.CHISQ.TEST(O3:P9,T3:U9)</f>
-        <v>2.3882165458915587E-8</v>
+        <v>2.3200456078028245E-12</v>
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="7">
+      <c r="B14" s="5">
         <v>202201</v>
       </c>
-      <c r="C14" s="7">
+      <c r="C14" s="5">
         <v>85</v>
       </c>
-      <c r="D14" s="7">
+      <c r="D14" s="5">
         <v>343</v>
       </c>
-      <c r="E14" s="7">
+      <c r="E14" s="5">
         <v>4.04</v>
       </c>
-      <c r="F14" s="7">
+      <c r="F14" s="5">
         <v>264</v>
       </c>
-      <c r="G14" s="10" t="s">
+      <c r="G14" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="H14" s="10" t="s">
+      <c r="H14" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="I14" s="13" t="s">
+      <c r="I14" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="J14" s="14" t="s">
+      <c r="J14" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="R14" s="20" t="s">
+      <c r="R14" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="S14" s="20"/>
+      <c r="S14" s="17"/>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A15" s="16" t="s">
+      <c r="A15" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="16">
+      <c r="B15" s="13">
         <v>202105</v>
       </c>
-      <c r="C15" s="16">
+      <c r="C15" s="13">
         <v>164</v>
       </c>
-      <c r="D15" s="16">
+      <c r="D15" s="13">
         <v>1109</v>
       </c>
-      <c r="E15" s="16">
+      <c r="E15" s="13">
         <v>6.76</v>
       </c>
-      <c r="F15" s="16">
+      <c r="F15" s="13">
         <v>831</v>
       </c>
-      <c r="G15" s="16">
+      <c r="G15" s="13">
         <v>61</v>
       </c>
-      <c r="H15" s="16">
+      <c r="H15" s="13">
         <v>52</v>
       </c>
-      <c r="I15" s="17">
+      <c r="I15" s="14">
         <v>7.3400000000000007E-2</v>
       </c>
-      <c r="J15" s="18">
+      <c r="J15" s="15">
         <v>0.85250000000000004</v>
       </c>
       <c r="N15" t="s">
@@ -2332,7 +2428,7 @@
       </c>
       <c r="O19">
         <f>SUM(G3:G8)-SUM(H3:H8)</f>
-        <v>94</v>
+        <v>142</v>
       </c>
       <c r="P19">
         <f>SUM(H3:H8)</f>
@@ -2340,22 +2436,22 @@
       </c>
       <c r="Q19">
         <f>SUM(O19:P19)</f>
-        <v>241</v>
+        <v>289</v>
       </c>
       <c r="S19" t="s">
         <v>12</v>
       </c>
       <c r="T19">
         <f>$Q19/$Q$22*O$22</f>
-        <v>92.083582089552237</v>
+        <v>132.80417754569191</v>
       </c>
       <c r="U19">
         <f>$Q19/$Q$22*P$22</f>
-        <v>148.91641791044776</v>
+        <v>156.19582245430809</v>
       </c>
       <c r="V19">
         <f>SUM(T19:U19)</f>
-        <v>241</v>
+        <v>289</v>
       </c>
     </row>
     <row r="20" spans="14:22" x14ac:dyDescent="0.3">
@@ -2379,11 +2475,11 @@
       </c>
       <c r="T20">
         <f t="shared" ref="T20:U21" si="6">$Q20/$Q$22*O$22</f>
-        <v>4.2029850746268655</v>
+        <v>5.0548302872062667</v>
       </c>
       <c r="U20">
         <f t="shared" si="6"/>
-        <v>6.7970149253731345</v>
+        <v>5.9451697127937342</v>
       </c>
       <c r="V20">
         <f t="shared" ref="V20:V21" si="7">SUM(T20:U20)</f>
@@ -2411,11 +2507,11 @@
       </c>
       <c r="T21">
         <f t="shared" si="6"/>
-        <v>31.713432835820896</v>
+        <v>38.140992167101828</v>
       </c>
       <c r="U21">
         <f t="shared" si="6"/>
-        <v>51.286567164179104</v>
+        <v>44.859007832898172</v>
       </c>
       <c r="V21">
         <f t="shared" si="7"/>
@@ -2425,7 +2521,7 @@
     <row r="22" spans="14:22" x14ac:dyDescent="0.3">
       <c r="O22">
         <f>SUM(O19:O21)</f>
-        <v>128</v>
+        <v>176</v>
       </c>
       <c r="P22">
         <f>SUM(P19:P21)</f>
@@ -2433,11 +2529,11 @@
       </c>
       <c r="Q22">
         <f>SUM(Q19:Q21)</f>
-        <v>335</v>
+        <v>383</v>
       </c>
       <c r="T22">
         <f>SUM(T19:T21)</f>
-        <v>128</v>
+        <v>176</v>
       </c>
       <c r="U22">
         <f>SUM(U19:U21)</f>
@@ -2445,7 +2541,7 @@
       </c>
       <c r="V22">
         <f>SUM(V19:V21)</f>
-        <v>335</v>
+        <v>383</v>
       </c>
     </row>
     <row r="25" spans="14:22" x14ac:dyDescent="0.3">
@@ -2454,7 +2550,7 @@
       </c>
       <c r="S25">
         <f>_xlfn.CHISQ.TEST(O19:P21,T19:U21)</f>
-        <v>0.36574017814468812</v>
+        <v>3.8891636613353403E-2</v>
       </c>
     </row>
     <row r="26" spans="14:22" x14ac:dyDescent="0.3">
@@ -2588,10 +2684,10 @@
       </c>
     </row>
     <row r="36" spans="14:22" x14ac:dyDescent="0.3">
-      <c r="R36" s="20" t="s">
+      <c r="R36" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="S36" s="20">
+      <c r="S36" s="17">
         <f>_xlfn.CHISQ.TEST(O32:P33,T32:U33)</f>
         <v>2.5124257489228916E-3</v>
       </c>
@@ -2702,7 +2798,7 @@
         <v>0</v>
       </c>
       <c r="Q47">
-        <f t="shared" ref="Q47:Q50" si="17">SUM(O47:P47)</f>
+        <f t="shared" ref="Q47:Q49" si="17">SUM(O47:P47)</f>
         <v>1</v>
       </c>
       <c r="S47" t="s">
@@ -2717,7 +2813,7 @@
         <v>0.66265060240963858</v>
       </c>
       <c r="V47">
-        <f t="shared" ref="V47:V50" si="18">SUM(T47:U47)</f>
+        <f t="shared" ref="V47:V49" si="18">SUM(T47:U47)</f>
         <v>1</v>
       </c>
     </row>
@@ -2769,7 +2865,7 @@
         <v>23</v>
       </c>
       <c r="T49">
-        <f t="shared" ref="T48:T49" si="20">$Q49/$Q$50*O$50</f>
+        <f t="shared" ref="T49" si="20">$Q49/$Q$50*O$50</f>
         <v>20.578313253012048</v>
       </c>
       <c r="U49">
@@ -2808,10 +2904,10 @@
       </c>
     </row>
     <row r="52" spans="14:22" x14ac:dyDescent="0.3">
-      <c r="R52" s="20" t="s">
+      <c r="R52" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="S52" s="20">
+      <c r="S52" s="17">
         <f>_xlfn.CHISQ.TEST(O47:P49,T47:U49)</f>
         <v>8.4563372478928258E-9</v>
       </c>

</xml_diff>

<commit_message>
table and doc updates
</commit_message>
<xml_diff>
--- a/docs/All_ves_by_npz_formatted_table.xlsx
+++ b/docs/All_ves_by_npz_formatted_table.xlsx
@@ -1,26 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jessica.mccordic.NMFS\Documents\GitHub\AMP_ves_summary\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jessica.mccordic\Documents\GitHub\AMP_ves_summary\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB95BFD2-5EDC-48BF-96C6-02B89A5C4E44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3000" windowWidth="16224" windowHeight="9108"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="All_ves_by_npz_formatted_table" sheetId="1" r:id="rId1"/>
     <sheet name="chisq" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="54">
   <si>
     <t>Network</t>
   </si>
@@ -147,12 +159,48 @@
   <si>
     <t>Deployment start 
 (mm/yyyy)</t>
+  </si>
+  <si>
+    <t>Range N vessels per day (min - max)</t>
+  </si>
+  <si>
+    <t>0 - 32</t>
+  </si>
+  <si>
+    <t>0 - 19</t>
+  </si>
+  <si>
+    <t>0 - 33</t>
+  </si>
+  <si>
+    <t>0 - 23</t>
+  </si>
+  <si>
+    <t>0 - 28</t>
+  </si>
+  <si>
+    <t>0 - 13</t>
+  </si>
+  <si>
+    <t>0 - 6</t>
+  </si>
+  <si>
+    <t>0 - 38</t>
+  </si>
+  <si>
+    <t>0 - 1</t>
+  </si>
+  <si>
+    <t>0 - 11</t>
+  </si>
+  <si>
+    <t>0 - 55</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="mm/yyyy"/>
@@ -745,7 +793,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
@@ -806,6 +854,9 @@
     </xf>
     <xf numFmtId="0" fontId="19" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -1128,27 +1179,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:Q15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B2:R15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="14.44140625" style="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" style="19"/>
-    <col min="4" max="4" width="27.33203125" style="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.44140625" style="19" customWidth="1"/>
-    <col min="6" max="6" width="8.6640625" style="19" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.77734375" style="19" customWidth="1"/>
-    <col min="9" max="9" width="12.5546875" customWidth="1"/>
-    <col min="10" max="10" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.453125" style="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.90625" style="19"/>
+    <col min="4" max="4" width="27.36328125" style="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.453125" style="19" customWidth="1"/>
+    <col min="6" max="6" width="8.6328125" style="19" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.6328125" style="19" customWidth="1"/>
+    <col min="8" max="8" width="8.81640625" style="19" customWidth="1"/>
+    <col min="10" max="10" width="12.54296875" customWidth="1"/>
+    <col min="11" max="11" width="13.6328125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:17" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:18" ht="37.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="23" t="s">
         <v>0</v>
       </c>
@@ -1165,25 +1217,28 @@
         <v>40</v>
       </c>
       <c r="G2" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="H2" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>6</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>7</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>8</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>9</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B3" s="28" t="s">
         <v>11</v>
       </c>
@@ -1199,27 +1254,30 @@
       <c r="F3" s="22">
         <v>364</v>
       </c>
-      <c r="G3" s="22">
+      <c r="G3" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="H3" s="22">
         <v>10.4</v>
       </c>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2">
+      <c r="I3" s="2"/>
+      <c r="J3" s="2">
         <v>208</v>
       </c>
-      <c r="J3" s="2">
+      <c r="K3" s="2">
         <v>41</v>
       </c>
-      <c r="K3" s="2">
-        <v>14</v>
-      </c>
-      <c r="L3" s="3">
+      <c r="L3" s="2">
+        <v>15</v>
+      </c>
+      <c r="M3" s="3">
         <v>0.197115384615384</v>
       </c>
-      <c r="M3" s="4">
+      <c r="N3" s="4">
         <v>0.36585365853658502</v>
       </c>
     </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B4" s="28"/>
       <c r="C4" s="26"/>
       <c r="D4" s="20">
@@ -1231,39 +1289,42 @@
       <c r="F4" s="22">
         <v>395</v>
       </c>
-      <c r="G4" s="22">
+      <c r="G4" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="H4" s="22">
         <v>5.56</v>
       </c>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5">
+      <c r="I4" s="5"/>
+      <c r="J4" s="5">
         <v>216</v>
       </c>
-      <c r="J4" s="5">
+      <c r="K4" s="5">
         <v>33</v>
       </c>
-      <c r="K4" s="5">
-        <v>0</v>
-      </c>
-      <c r="L4" s="6">
+      <c r="L4" s="5">
+        <v>22</v>
+      </c>
+      <c r="M4" s="6">
         <v>0.15277777777777701</v>
       </c>
-      <c r="M4" s="16">
+      <c r="N4" s="16">
         <v>0.66666666666666596</v>
-      </c>
-      <c r="O4">
-        <f>SUM(I3:I5)</f>
-        <v>750</v>
       </c>
       <c r="P4">
         <f>SUM(J3:J5)</f>
+        <v>750</v>
+      </c>
+      <c r="Q4">
+        <f>SUM(K3:K5)</f>
         <v>131</v>
       </c>
-      <c r="Q4">
-        <f>P4/O4</f>
+      <c r="R4">
+        <f>Q4/P4</f>
         <v>0.17466666666666666</v>
       </c>
     </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B5" s="28"/>
       <c r="C5" s="27"/>
       <c r="D5" s="20">
@@ -1275,27 +1336,30 @@
       <c r="F5" s="22">
         <v>473</v>
       </c>
-      <c r="G5" s="22">
+      <c r="G5" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="H5" s="22">
         <v>6.31</v>
       </c>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5">
+      <c r="I5" s="5"/>
+      <c r="J5" s="5">
         <v>326</v>
       </c>
-      <c r="J5" s="5">
+      <c r="K5" s="5">
         <v>57</v>
       </c>
-      <c r="K5" s="5">
-        <v>31</v>
-      </c>
-      <c r="L5" s="6">
+      <c r="L5" s="5">
+        <v>33</v>
+      </c>
+      <c r="M5" s="6">
         <v>0.17484662576687099</v>
       </c>
-      <c r="M5" s="7">
+      <c r="N5" s="7">
         <v>0.57894736842105199</v>
       </c>
     </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B6" s="28"/>
       <c r="C6" s="26" t="s">
         <v>14</v>
@@ -1309,27 +1373,30 @@
       <c r="F6" s="22">
         <v>523</v>
       </c>
-      <c r="G6" s="22">
+      <c r="G6" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="H6" s="22">
         <v>7.81</v>
       </c>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5">
+      <c r="I6" s="5"/>
+      <c r="J6" s="5">
         <v>112</v>
       </c>
-      <c r="J6" s="5">
+      <c r="K6" s="5">
         <v>41</v>
       </c>
-      <c r="K6" s="5">
-        <v>8</v>
-      </c>
-      <c r="L6" s="6">
+      <c r="L6" s="5">
+        <v>12</v>
+      </c>
+      <c r="M6" s="6">
         <v>0.36607142857142799</v>
       </c>
-      <c r="M6" s="7">
+      <c r="N6" s="7">
         <v>0.292682926829268</v>
       </c>
     </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B7" s="28"/>
       <c r="C7" s="26"/>
       <c r="D7" s="20">
@@ -1341,39 +1408,42 @@
       <c r="F7" s="22">
         <v>443</v>
       </c>
-      <c r="G7" s="22">
+      <c r="G7" s="31" t="s">
+        <v>46</v>
+      </c>
+      <c r="H7" s="22">
         <v>6.33</v>
       </c>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5">
+      <c r="I7" s="5"/>
+      <c r="J7" s="5">
         <v>265</v>
       </c>
-      <c r="J7" s="5">
+      <c r="K7" s="5">
         <v>42</v>
       </c>
-      <c r="K7" s="5">
-        <v>29</v>
-      </c>
-      <c r="L7" s="6">
+      <c r="L7" s="5">
+        <v>30</v>
+      </c>
+      <c r="M7" s="6">
         <v>0.15849056603773501</v>
       </c>
-      <c r="M7" s="7">
+      <c r="N7" s="7">
         <v>0.71428571428571397</v>
-      </c>
-      <c r="O7">
-        <f>SUM(I6:I8)</f>
-        <v>618</v>
       </c>
       <c r="P7">
         <f>SUM(J6:J8)</f>
+        <v>618</v>
+      </c>
+      <c r="Q7">
+        <f>SUM(K6:K8)</f>
         <v>158</v>
       </c>
-      <c r="Q7">
-        <f>P7/O7</f>
+      <c r="R7">
+        <f>Q7/P7</f>
         <v>0.25566343042071199</v>
       </c>
     </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B8" s="29"/>
       <c r="C8" s="27"/>
       <c r="D8" s="20">
@@ -1385,28 +1455,31 @@
       <c r="F8" s="22">
         <v>343</v>
       </c>
-      <c r="G8" s="22">
+      <c r="G8" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="H8" s="22">
         <v>4.2300000000000004</v>
       </c>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13">
+      <c r="I8" s="13"/>
+      <c r="J8" s="13">
         <v>241</v>
       </c>
-      <c r="J8" s="13">
+      <c r="K8" s="13">
         <v>75</v>
       </c>
-      <c r="K8" s="13">
-        <v>65</v>
-      </c>
-      <c r="L8" s="14">
+      <c r="L8" s="13">
+        <v>68</v>
+      </c>
+      <c r="M8" s="14">
         <v>0.31120331950207403</v>
       </c>
-      <c r="M8" s="15">
+      <c r="N8" s="15">
         <v>0.90666666666666595</v>
       </c>
-      <c r="N8" s="1"/>
-    </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="O8" s="1"/>
+    </row>
+    <row r="9" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B9" s="30" t="s">
         <v>15</v>
       </c>
@@ -1422,27 +1495,30 @@
       <c r="F9" s="22">
         <v>376</v>
       </c>
-      <c r="G9" s="22">
+      <c r="G9" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="H9" s="22">
         <v>3.24</v>
       </c>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2">
+      <c r="I9" s="2"/>
+      <c r="J9" s="2">
         <v>125</v>
       </c>
-      <c r="J9" s="2">
+      <c r="K9" s="2">
         <v>7</v>
       </c>
-      <c r="K9" s="2">
+      <c r="L9" s="2">
         <v>3</v>
       </c>
-      <c r="L9" s="3">
+      <c r="M9" s="3">
         <v>5.6000000000000001E-2</v>
       </c>
-      <c r="M9" s="4">
+      <c r="N9" s="4">
         <v>0.42859999999999998</v>
       </c>
     </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B10" s="29"/>
       <c r="C10" s="24" t="s">
         <v>17</v>
@@ -1456,27 +1532,30 @@
       <c r="F10" s="22">
         <v>126</v>
       </c>
-      <c r="G10" s="22">
+      <c r="G10" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="H10" s="22">
         <v>1.1399999999999999</v>
       </c>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13">
+      <c r="I10" s="13"/>
+      <c r="J10" s="13">
         <v>109</v>
       </c>
-      <c r="J10" s="13">
+      <c r="K10" s="13">
         <v>4</v>
       </c>
-      <c r="K10" s="13">
+      <c r="L10" s="13">
         <v>2</v>
       </c>
-      <c r="L10" s="14">
+      <c r="M10" s="14">
         <v>3.6700000000000003E-2</v>
       </c>
-      <c r="M10" s="15">
+      <c r="N10" s="15">
         <v>0.5</v>
       </c>
     </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B11" s="30" t="s">
         <v>18</v>
       </c>
@@ -1492,27 +1571,30 @@
       <c r="F11" s="22">
         <v>575</v>
       </c>
-      <c r="G11" s="22">
+      <c r="G11" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="H11" s="22">
         <v>6.32</v>
       </c>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2">
+      <c r="I11" s="2"/>
+      <c r="J11" s="2">
         <v>390</v>
       </c>
-      <c r="J11" s="2">
+      <c r="K11" s="2">
         <v>1</v>
       </c>
-      <c r="K11" s="2">
+      <c r="L11" s="2">
         <v>0</v>
       </c>
-      <c r="L11" s="3">
+      <c r="M11" s="3">
         <v>2.5999999999999999E-3</v>
       </c>
-      <c r="M11" s="4">
+      <c r="N11" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B12" s="28"/>
       <c r="C12" s="24" t="s">
         <v>20</v>
@@ -1526,27 +1608,30 @@
       <c r="F12" s="22">
         <v>425</v>
       </c>
-      <c r="G12" s="22">
+      <c r="G12" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="H12" s="22">
         <v>4.01</v>
       </c>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5">
+      <c r="I12" s="5"/>
+      <c r="J12" s="5">
         <v>345</v>
       </c>
-      <c r="J12" s="5">
+      <c r="K12" s="5">
         <v>21</v>
       </c>
-      <c r="K12" s="5">
+      <c r="L12" s="5">
         <v>3</v>
       </c>
-      <c r="L12" s="6">
+      <c r="M12" s="6">
         <v>6.0900000000000003E-2</v>
       </c>
-      <c r="M12" s="7">
+      <c r="N12" s="7">
         <v>0.1429</v>
       </c>
     </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B13" s="28"/>
       <c r="C13" s="24" t="s">
         <v>21</v>
@@ -1560,27 +1645,30 @@
       <c r="F13" s="22">
         <v>4</v>
       </c>
-      <c r="G13" s="22">
+      <c r="G13" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="H13" s="22">
         <v>0.02</v>
       </c>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5">
+      <c r="I13" s="5"/>
+      <c r="J13" s="5">
         <v>2</v>
-      </c>
-      <c r="J13" s="8" t="s">
-        <v>13</v>
       </c>
       <c r="K13" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="L13" s="9" t="s">
+      <c r="L13" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="M13" s="10" t="s">
+      <c r="M13" s="9" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="N13" s="10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B14" s="28"/>
       <c r="C14" s="24" t="s">
         <v>22</v>
@@ -1594,27 +1682,30 @@
       <c r="F14" s="22">
         <v>343</v>
       </c>
-      <c r="G14" s="22">
+      <c r="G14" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="H14" s="22">
         <v>4.04</v>
       </c>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5">
+      <c r="I14" s="5"/>
+      <c r="J14" s="5">
         <v>264</v>
-      </c>
-      <c r="J14" s="8" t="s">
-        <v>13</v>
       </c>
       <c r="K14" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="L14" s="11" t="s">
+      <c r="L14" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="M14" s="12" t="s">
+      <c r="M14" s="11" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="N14" s="12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B15" s="29"/>
       <c r="C15" s="24" t="s">
         <v>23</v>
@@ -1628,23 +1719,26 @@
       <c r="F15" s="22">
         <v>1109</v>
       </c>
-      <c r="G15" s="22">
+      <c r="G15" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="H15" s="22">
         <v>6.76</v>
       </c>
-      <c r="H15" s="13"/>
-      <c r="I15" s="13">
+      <c r="I15" s="13"/>
+      <c r="J15" s="13">
         <v>831</v>
       </c>
-      <c r="J15" s="13">
+      <c r="K15" s="13">
         <v>61</v>
       </c>
-      <c r="K15" s="13">
+      <c r="L15" s="13">
         <v>52</v>
       </c>
-      <c r="L15" s="14">
+      <c r="M15" s="14">
         <v>7.3400000000000007E-2</v>
       </c>
-      <c r="M15" s="15">
+      <c r="N15" s="15">
         <v>0.85250000000000004</v>
       </c>
     </row>
@@ -1656,7 +1750,7 @@
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="B11:B15"/>
   </mergeCells>
-  <conditionalFormatting sqref="L3:L15">
+  <conditionalFormatting sqref="M3:M15">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -1668,7 +1762,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M3:M12 M14:M15">
+  <conditionalFormatting sqref="N3:N12 N14:N15">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -1685,24 +1779,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:V52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:J15"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="T11" sqref="T11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="5" max="5" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="35.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.109375" customWidth="1"/>
+    <col min="5" max="5" width="13.08984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.90625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.6328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.6328125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.08984375" customWidth="1"/>
     <col min="19" max="19" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.35">
       <c r="N1" t="s">
         <v>27</v>
       </c>
@@ -1710,7 +1804,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1766,7 +1860,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -1789,7 +1883,7 @@
         <v>41</v>
       </c>
       <c r="H3" s="2">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I3" s="18">
         <v>0.197115384615384</v>
@@ -1802,11 +1896,11 @@
       </c>
       <c r="O3">
         <f>SUM(G3:G5)-SUM(H3:H5)</f>
-        <v>86</v>
+        <v>61</v>
       </c>
       <c r="P3">
         <f>SUM(H3:H5)</f>
-        <v>45</v>
+        <v>70</v>
       </c>
       <c r="Q3">
         <f>SUM(O3:P3)</f>
@@ -1817,18 +1911,18 @@
       </c>
       <c r="T3">
         <f>$Q3/$Q$10*O$10</f>
-        <v>60.198433420365532</v>
+        <v>48.911227154046998</v>
       </c>
       <c r="U3">
         <f>$Q3/$Q$10*P$10</f>
-        <v>70.801566579634468</v>
+        <v>82.088772845953002</v>
       </c>
       <c r="V3">
         <f>SUM(T3:U3)</f>
         <v>131</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A4" s="5"/>
       <c r="B4" s="5">
         <v>201812</v>
@@ -1849,7 +1943,7 @@
         <v>33</v>
       </c>
       <c r="H4" s="5">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="I4" s="18">
         <v>0.15277777777777701</v>
@@ -1862,11 +1956,11 @@
       </c>
       <c r="O4">
         <f>SUM(G6:G8)-SUM(H6:H8)</f>
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="P4">
         <f>SUM(H6:H8)</f>
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="Q4">
         <f t="shared" ref="Q4:Q9" si="0">SUM(O4:P4)</f>
@@ -1877,18 +1971,18 @@
       </c>
       <c r="T4">
         <f t="shared" ref="T4:U9" si="1">$Q4/$Q$10*O$10</f>
-        <v>72.605744125326368</v>
+        <v>58.992167101827675</v>
       </c>
       <c r="U4">
         <f t="shared" si="1"/>
-        <v>85.394255874673632</v>
+        <v>99.007832898172325</v>
       </c>
       <c r="V4">
         <f t="shared" ref="V4:V9" si="2">SUM(T4:U4)</f>
         <v>158</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A5" s="5"/>
       <c r="B5" s="5">
         <v>201904</v>
@@ -1909,7 +2003,7 @@
         <v>57</v>
       </c>
       <c r="H5" s="5">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="I5" s="18">
         <v>0.17484662576687099</v>
@@ -1935,18 +2029,18 @@
       </c>
       <c r="T5">
         <f t="shared" si="1"/>
-        <v>3.2167101827676241</v>
+        <v>2.6135770234986948</v>
       </c>
       <c r="U5">
         <f t="shared" si="1"/>
-        <v>3.7832898172323763</v>
+        <v>4.3864229765013061</v>
       </c>
       <c r="V5">
         <f t="shared" si="2"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+        <v>7.0000000000000009</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>14</v>
       </c>
@@ -1969,7 +2063,7 @@
         <v>41</v>
       </c>
       <c r="H6" s="5">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="I6" s="18">
         <v>0.36607142857142799</v>
@@ -1995,18 +2089,18 @@
       </c>
       <c r="T6">
         <f t="shared" si="1"/>
-        <v>1.8381201044386424</v>
+        <v>1.4934725848563968</v>
       </c>
       <c r="U6">
         <f t="shared" si="1"/>
-        <v>2.1618798955613578</v>
+        <v>2.5065274151436032</v>
       </c>
       <c r="V6">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A7" s="5"/>
       <c r="B7" s="5">
         <v>201812</v>
@@ -2027,7 +2121,7 @@
         <v>42</v>
       </c>
       <c r="H7" s="5">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I7" s="18">
         <v>0.15849056603773501</v>
@@ -2053,18 +2147,18 @@
       </c>
       <c r="T7">
         <f t="shared" si="1"/>
-        <v>0.45953002610966059</v>
+        <v>0.37336814621409919</v>
       </c>
       <c r="U7">
         <f t="shared" si="1"/>
-        <v>0.54046997389033946</v>
+        <v>0.62663185378590081</v>
       </c>
       <c r="V7">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A8" s="13"/>
       <c r="B8" s="13">
         <v>201906</v>
@@ -2085,7 +2179,7 @@
         <v>75</v>
       </c>
       <c r="H8" s="13">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="I8" s="18">
         <v>0.31120331950207403</v>
@@ -2111,18 +2205,18 @@
       </c>
       <c r="T8">
         <f t="shared" si="1"/>
-        <v>9.6501305483028723</v>
+        <v>7.8407310704960844</v>
       </c>
       <c r="U8">
         <f t="shared" si="1"/>
-        <v>11.349869451697129</v>
+        <v>13.159268929503916</v>
       </c>
       <c r="V8">
         <f t="shared" si="2"/>
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
@@ -2171,18 +2265,18 @@
       </c>
       <c r="T9">
         <f t="shared" si="1"/>
-        <v>28.031331592689295</v>
+        <v>22.775456919060051</v>
       </c>
       <c r="U9">
         <f t="shared" si="1"/>
-        <v>32.968668407310702</v>
+        <v>38.224543080939945</v>
       </c>
       <c r="V9">
         <f t="shared" si="2"/>
         <v>61</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A10" s="13" t="s">
         <v>17</v>
       </c>
@@ -2215,11 +2309,11 @@
       </c>
       <c r="O10">
         <f>SUM(O3:O9)</f>
-        <v>176</v>
+        <v>143</v>
       </c>
       <c r="P10">
         <f t="shared" ref="P10:Q10" si="3">SUM(P3:P9)</f>
-        <v>207</v>
+        <v>240</v>
       </c>
       <c r="Q10">
         <f t="shared" si="3"/>
@@ -2227,18 +2321,18 @@
       </c>
       <c r="T10">
         <f>SUM(T3:T9)</f>
-        <v>176.00000000000003</v>
+        <v>143</v>
       </c>
       <c r="U10">
         <f t="shared" ref="U10:V10" si="4">SUM(U3:U9)</f>
-        <v>206.99999999999997</v>
+        <v>240.00000000000003</v>
       </c>
       <c r="V10">
         <f t="shared" si="4"/>
         <v>383</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>19</v>
       </c>
@@ -2270,7 +2364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>20</v>
       </c>
@@ -2302,7 +2396,7 @@
         <v>0.1429</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>21</v>
       </c>
@@ -2338,10 +2432,10 @@
       </c>
       <c r="S13" s="17">
         <f>_xlfn.CHISQ.TEST(O3:P9,T3:U9)</f>
-        <v>2.3200456078028245E-12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
+        <v>3.781609838505567E-8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
         <v>22</v>
       </c>
@@ -2377,7 +2471,7 @@
       </c>
       <c r="S14" s="17"/>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A15" s="13" t="s">
         <v>23</v>
       </c>
@@ -2412,7 +2506,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="14:22" x14ac:dyDescent="0.3">
+    <row r="17" spans="14:22" x14ac:dyDescent="0.35">
       <c r="N17" t="s">
         <v>27</v>
       </c>
@@ -2420,7 +2514,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="14:22" x14ac:dyDescent="0.3">
+    <row r="18" spans="14:22" x14ac:dyDescent="0.35">
       <c r="N18" t="s">
         <v>1</v>
       </c>
@@ -2446,17 +2540,17 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="14:22" x14ac:dyDescent="0.3">
+    <row r="19" spans="14:22" x14ac:dyDescent="0.35">
       <c r="N19" t="s">
         <v>31</v>
       </c>
       <c r="O19">
         <f>SUM(G3:G8)-SUM(H3:H8)</f>
-        <v>142</v>
+        <v>109</v>
       </c>
       <c r="P19">
         <f>SUM(H3:H8)</f>
-        <v>147</v>
+        <v>180</v>
       </c>
       <c r="Q19">
         <f>SUM(O19:P19)</f>
@@ -2467,18 +2561,18 @@
       </c>
       <c r="T19">
         <f>$Q19/$Q$22*O$22</f>
-        <v>132.80417754569191</v>
+        <v>107.90339425587467</v>
       </c>
       <c r="U19">
         <f>$Q19/$Q$22*P$22</f>
-        <v>156.19582245430809</v>
+        <v>181.09660574412533</v>
       </c>
       <c r="V19">
         <f>SUM(T19:U19)</f>
         <v>289</v>
       </c>
     </row>
-    <row r="20" spans="14:22" x14ac:dyDescent="0.3">
+    <row r="20" spans="14:22" x14ac:dyDescent="0.35">
       <c r="N20" t="s">
         <v>15</v>
       </c>
@@ -2499,18 +2593,18 @@
       </c>
       <c r="T20">
         <f t="shared" ref="T20:U21" si="6">$Q20/$Q$22*O$22</f>
-        <v>5.0548302872062667</v>
+        <v>4.1070496083550916</v>
       </c>
       <c r="U20">
         <f t="shared" si="6"/>
-        <v>5.9451697127937342</v>
+        <v>6.8929503916449093</v>
       </c>
       <c r="V20">
         <f t="shared" ref="V20:V21" si="7">SUM(T20:U20)</f>
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="14:22" x14ac:dyDescent="0.3">
+    <row r="21" spans="14:22" x14ac:dyDescent="0.35">
       <c r="N21" t="s">
         <v>32</v>
       </c>
@@ -2531,25 +2625,25 @@
       </c>
       <c r="T21">
         <f t="shared" si="6"/>
-        <v>38.140992167101828</v>
+        <v>30.989556135770236</v>
       </c>
       <c r="U21">
         <f t="shared" si="6"/>
-        <v>44.859007832898172</v>
+        <v>52.010443864229764</v>
       </c>
       <c r="V21">
         <f t="shared" si="7"/>
         <v>83</v>
       </c>
     </row>
-    <row r="22" spans="14:22" x14ac:dyDescent="0.3">
+    <row r="22" spans="14:22" x14ac:dyDescent="0.35">
       <c r="O22">
         <f>SUM(O19:O21)</f>
-        <v>176</v>
+        <v>143</v>
       </c>
       <c r="P22">
         <f>SUM(P19:P21)</f>
-        <v>207</v>
+        <v>240</v>
       </c>
       <c r="Q22">
         <f>SUM(Q19:Q21)</f>
@@ -2557,37 +2651,37 @@
       </c>
       <c r="T22">
         <f>SUM(T19:T21)</f>
-        <v>176</v>
+        <v>143</v>
       </c>
       <c r="U22">
         <f>SUM(U19:U21)</f>
-        <v>207</v>
+        <v>240</v>
       </c>
       <c r="V22">
         <f>SUM(V19:V21)</f>
         <v>383</v>
       </c>
     </row>
-    <row r="25" spans="14:22" x14ac:dyDescent="0.3">
+    <row r="25" spans="14:22" x14ac:dyDescent="0.35">
       <c r="R25" t="s">
         <v>35</v>
       </c>
       <c r="S25">
         <f>_xlfn.CHISQ.TEST(O19:P21,T19:U21)</f>
-        <v>3.8891636613353403E-2</v>
-      </c>
-    </row>
-    <row r="26" spans="14:22" x14ac:dyDescent="0.3">
+        <v>0.39251979118350044</v>
+      </c>
+    </row>
+    <row r="26" spans="14:22" x14ac:dyDescent="0.35">
       <c r="R26" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="14:22" x14ac:dyDescent="0.3">
+    <row r="28" spans="14:22" x14ac:dyDescent="0.35">
       <c r="N28" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="30" spans="14:22" x14ac:dyDescent="0.3">
+    <row r="30" spans="14:22" x14ac:dyDescent="0.35">
       <c r="N30" t="s">
         <v>27</v>
       </c>
@@ -2595,7 +2689,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="14:22" x14ac:dyDescent="0.3">
+    <row r="31" spans="14:22" x14ac:dyDescent="0.35">
       <c r="N31" t="s">
         <v>1</v>
       </c>
@@ -2621,102 +2715,100 @@
         <v>26</v>
       </c>
     </row>
-    <row r="32" spans="14:22" x14ac:dyDescent="0.3">
+    <row r="32" spans="14:22" x14ac:dyDescent="0.35">
       <c r="N32" t="s">
         <v>12</v>
       </c>
       <c r="O32">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="P32">
-        <v>45</v>
+        <v>70</v>
       </c>
       <c r="Q32">
-        <f>SUM(O32:P32)</f>
-        <v>92</v>
+        <v>131</v>
       </c>
       <c r="S32" t="s">
         <v>12</v>
       </c>
       <c r="T32">
         <f>$Q32/$Q$34*O$34</f>
-        <v>35.883817427385893</v>
+        <v>49.408304498269899</v>
       </c>
       <c r="U32">
         <f>$Q32/$Q$34*P$34</f>
-        <v>56.116182572614107</v>
+        <v>81.591695501730101</v>
       </c>
       <c r="V32">
         <f>SUM(T32:U32)</f>
-        <v>92</v>
-      </c>
-    </row>
-    <row r="33" spans="14:22" x14ac:dyDescent="0.3">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="33" spans="14:22" x14ac:dyDescent="0.35">
       <c r="N33" t="s">
         <v>14</v>
       </c>
       <c r="O33">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="P33">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="Q33">
-        <f t="shared" ref="Q33" si="8">SUM(O33:P33)</f>
-        <v>149</v>
+        <v>158</v>
       </c>
       <c r="S33" t="s">
         <v>14</v>
       </c>
       <c r="T33">
         <f>$Q33/$Q$34*O$34</f>
-        <v>58.116182572614107</v>
+        <v>59.591695501730108</v>
       </c>
       <c r="U33">
         <f>$Q33/$Q$34*P$34</f>
-        <v>90.883817427385893</v>
+        <v>98.408304498269899</v>
       </c>
       <c r="V33">
-        <f t="shared" ref="V33" si="9">SUM(T33:U33)</f>
-        <v>149</v>
-      </c>
-    </row>
-    <row r="34" spans="14:22" x14ac:dyDescent="0.3">
+        <f t="shared" ref="V33" si="8">SUM(T33:U33)</f>
+        <v>158</v>
+      </c>
+    </row>
+    <row r="34" spans="14:22" x14ac:dyDescent="0.35">
       <c r="O34">
         <f>SUM(O32:O33)</f>
-        <v>94</v>
+        <v>109</v>
       </c>
       <c r="P34">
-        <f t="shared" ref="P34:Q34" si="10">SUM(P32:P33)</f>
-        <v>147</v>
+        <f t="shared" ref="P34:Q34" si="9">SUM(P32:P33)</f>
+        <v>180</v>
       </c>
       <c r="Q34">
-        <f t="shared" si="10"/>
-        <v>241</v>
+        <f t="shared" si="9"/>
+        <v>289</v>
       </c>
       <c r="T34">
         <f>SUM(T32:T33)</f>
-        <v>94</v>
+        <v>109</v>
       </c>
       <c r="U34">
-        <f t="shared" ref="U34:V34" si="11">SUM(U32:U33)</f>
-        <v>147</v>
+        <f t="shared" ref="U34:V34" si="10">SUM(U32:U33)</f>
+        <v>180</v>
       </c>
       <c r="V34">
-        <f t="shared" si="11"/>
-        <v>241</v>
-      </c>
-    </row>
-    <row r="36" spans="14:22" x14ac:dyDescent="0.3">
+        <f t="shared" si="10"/>
+        <v>289</v>
+      </c>
+    </row>
+    <row r="36" spans="14:22" x14ac:dyDescent="0.35">
       <c r="R36" s="17" t="s">
         <v>37</v>
       </c>
       <c r="S36" s="17">
         <f>_xlfn.CHISQ.TEST(O32:P33,T32:U33)</f>
-        <v>2.5124257489228916E-3</v>
-      </c>
-    </row>
-    <row r="40" spans="14:22" x14ac:dyDescent="0.3">
+        <v>4.712572141964003E-3</v>
+      </c>
+    </row>
+    <row r="40" spans="14:22" x14ac:dyDescent="0.35">
       <c r="N40" t="s">
         <v>16</v>
       </c>
@@ -2727,7 +2819,7 @@
         <v>3</v>
       </c>
       <c r="Q40">
-        <f t="shared" ref="Q40:Q41" si="12">SUM(O40:P40)</f>
+        <f t="shared" ref="Q40:Q41" si="11">SUM(O40:P40)</f>
         <v>7</v>
       </c>
       <c r="S40" t="s">
@@ -2746,7 +2838,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="14:22" x14ac:dyDescent="0.3">
+    <row r="41" spans="14:22" x14ac:dyDescent="0.35">
       <c r="N41" t="s">
         <v>17</v>
       </c>
@@ -2757,7 +2849,7 @@
         <v>2</v>
       </c>
       <c r="Q41">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>4</v>
       </c>
       <c r="S41" t="s">
@@ -2772,21 +2864,21 @@
         <v>1.8181818181818183</v>
       </c>
       <c r="V41">
-        <f t="shared" ref="V41" si="13">SUM(T41:U41)</f>
+        <f t="shared" ref="V41" si="12">SUM(T41:U41)</f>
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="14:22" x14ac:dyDescent="0.3">
+    <row r="42" spans="14:22" x14ac:dyDescent="0.35">
       <c r="O42">
         <f>SUM(O40:O41)</f>
         <v>6</v>
       </c>
       <c r="P42">
-        <f t="shared" ref="P42:Q42" si="14">SUM(P40:P41)</f>
+        <f t="shared" ref="P42:Q42" si="13">SUM(P40:P41)</f>
         <v>5</v>
       </c>
       <c r="Q42">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>11</v>
       </c>
       <c r="T42">
@@ -2794,15 +2886,15 @@
         <v>6</v>
       </c>
       <c r="U42">
-        <f t="shared" ref="U42" si="15">SUM(U40:U41)</f>
+        <f t="shared" ref="U42" si="14">SUM(U40:U41)</f>
         <v>5</v>
       </c>
       <c r="V42">
-        <f t="shared" ref="V42" si="16">SUM(V40:V41)</f>
+        <f t="shared" ref="V42" si="15">SUM(V40:V41)</f>
         <v>11</v>
       </c>
     </row>
-    <row r="44" spans="14:22" x14ac:dyDescent="0.3">
+    <row r="44" spans="14:22" x14ac:dyDescent="0.35">
       <c r="R44" t="s">
         <v>38</v>
       </c>
@@ -2811,7 +2903,7 @@
         <v>0.81897084890175897</v>
       </c>
     </row>
-    <row r="47" spans="14:22" x14ac:dyDescent="0.3">
+    <row r="47" spans="14:22" x14ac:dyDescent="0.35">
       <c r="N47" t="s">
         <v>19</v>
       </c>
@@ -2822,7 +2914,7 @@
         <v>0</v>
       </c>
       <c r="Q47">
-        <f t="shared" ref="Q47:Q49" si="17">SUM(O47:P47)</f>
+        <f t="shared" ref="Q47:Q49" si="16">SUM(O47:P47)</f>
         <v>1</v>
       </c>
       <c r="S47" t="s">
@@ -2837,11 +2929,11 @@
         <v>0.66265060240963858</v>
       </c>
       <c r="V47">
-        <f t="shared" ref="V47:V49" si="18">SUM(T47:U47)</f>
+        <f t="shared" ref="V47:V49" si="17">SUM(T47:U47)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="14:22" x14ac:dyDescent="0.3">
+    <row r="48" spans="14:22" x14ac:dyDescent="0.35">
       <c r="N48" t="s">
         <v>20</v>
       </c>
@@ -2852,7 +2944,7 @@
         <v>3</v>
       </c>
       <c r="Q48">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>21</v>
       </c>
       <c r="S48" t="s">
@@ -2863,15 +2955,15 @@
         <v>7.0843373493975896</v>
       </c>
       <c r="U48">
-        <f t="shared" ref="U48:U49" si="19">$Q48/$Q$50*P$50</f>
+        <f t="shared" ref="U48:U49" si="18">$Q48/$Q$50*P$50</f>
         <v>13.915662650602409</v>
       </c>
       <c r="V48">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v>21</v>
       </c>
     </row>
-    <row r="49" spans="14:22" x14ac:dyDescent="0.3">
+    <row r="49" spans="14:22" x14ac:dyDescent="0.35">
       <c r="N49" t="s">
         <v>23</v>
       </c>
@@ -2882,36 +2974,36 @@
         <v>52</v>
       </c>
       <c r="Q49">
+        <f t="shared" si="16"/>
+        <v>61</v>
+      </c>
+      <c r="S49" t="s">
+        <v>23</v>
+      </c>
+      <c r="T49">
+        <f t="shared" ref="T49" si="19">$Q49/$Q$50*O$50</f>
+        <v>20.578313253012048</v>
+      </c>
+      <c r="U49">
+        <f t="shared" si="18"/>
+        <v>40.421686746987952</v>
+      </c>
+      <c r="V49">
         <f t="shared" si="17"/>
         <v>61</v>
       </c>
-      <c r="S49" t="s">
-        <v>23</v>
-      </c>
-      <c r="T49">
-        <f t="shared" ref="T49" si="20">$Q49/$Q$50*O$50</f>
-        <v>20.578313253012048</v>
-      </c>
-      <c r="U49">
-        <f t="shared" si="19"/>
-        <v>40.421686746987952</v>
-      </c>
-      <c r="V49">
-        <f t="shared" si="18"/>
-        <v>61</v>
-      </c>
-    </row>
-    <row r="50" spans="14:22" x14ac:dyDescent="0.3">
+    </row>
+    <row r="50" spans="14:22" x14ac:dyDescent="0.35">
       <c r="O50">
         <f>SUM(O47:O49)</f>
         <v>28</v>
       </c>
       <c r="P50">
-        <f t="shared" ref="P50:Q50" si="21">SUM(P47:P49)</f>
+        <f t="shared" ref="P50:Q50" si="20">SUM(P47:P49)</f>
         <v>55</v>
       </c>
       <c r="Q50">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v>83</v>
       </c>
       <c r="T50">
@@ -2919,15 +3011,15 @@
         <v>28</v>
       </c>
       <c r="U50">
-        <f t="shared" ref="U50:V50" si="22">SUM(U43:U49)</f>
+        <f t="shared" ref="U50:V50" si="21">SUM(U43:U49)</f>
         <v>55</v>
       </c>
       <c r="V50">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>83</v>
       </c>
     </row>
-    <row r="52" spans="14:22" x14ac:dyDescent="0.3">
+    <row r="52" spans="14:22" x14ac:dyDescent="0.35">
       <c r="R52" s="17" t="s">
         <v>39</v>
       </c>

</xml_diff>